<commit_message>
Converted updated Localization spreadsheet
</commit_message>
<xml_diff>
--- a/Assets/Resources/LocalizationEntry.xlsx
+++ b/Assets/Resources/LocalizationEntry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonjaunger/Documents/GitHub/OctaviCopterFestival/Assets/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProjects\OctaviCopterFestival\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5DF599-D2EF-3547-A236-C6B3417D742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A2F406-EF35-44D8-9E9D-F20F54B9F240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2660" yWindow="-22520" windowWidth="35840" windowHeight="20920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocalizationEntry" sheetId="1" r:id="rId1"/>
@@ -281,15 +281,9 @@
     <t>Steer with your head</t>
   </si>
   <si>
-    <t>(       ) start/pause/resume game</t>
-  </si>
-  <si>
     <t>Green buttons replay the hint</t>
   </si>
   <si>
-    <t>(F) (       ) start/pause/resume game</t>
-  </si>
-  <si>
     <t>IAALevel1Name</t>
   </si>
   <si>
@@ -398,9 +392,6 @@
     <t>Die grünen Knöpfe wiederholen die zu treffenden Töne</t>
   </si>
   <si>
-    <t>(       ) Start/Pause</t>
-  </si>
-  <si>
     <t>Zurück</t>
   </si>
   <si>
@@ -473,9 +464,6 @@
     <t>Botones verdesc repiten las notas a tocar</t>
   </si>
   <si>
-    <t>(       ) comenzar/pausar/resumir juego</t>
-  </si>
-  <si>
     <t>Regresar</t>
   </si>
   <si>
@@ -522,6 +510,18 @@
   </si>
   <si>
     <t>Vamo' arriba!</t>
+  </si>
+  <si>
+    <t>(  &lt;sprite name="FlatHamburger" ) start/pause/resume game</t>
+  </si>
+  <si>
+    <t>(  &lt;sprite name="FlatHamburger" ) Start/Pause</t>
+  </si>
+  <si>
+    <t>(  &lt;sprite name="FlatHamburger" ) comenzar/pausar/resumir juego</t>
+  </si>
+  <si>
+    <t>(F) (  &lt;sprite name="FlatHamburger" ) start/pause/resume game</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -841,20 +841,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="66.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
     <col min="4" max="4" width="96" customWidth="1"/>
-    <col min="5" max="5" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>40</v>
       </c>
@@ -868,7 +868,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -876,33 +876,33 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -910,16 +910,16 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -927,16 +927,16 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -944,16 +944,16 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -961,16 +961,16 @@
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -978,16 +978,16 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -995,16 +995,16 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -1021,7 +1021,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1029,16 +1029,16 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1046,16 +1046,16 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1063,16 +1063,16 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1080,16 +1080,16 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1100,13 +1100,13 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1114,16 +1114,16 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1134,13 +1134,13 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1148,16 +1148,16 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1165,16 +1165,16 @@
         <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1182,16 +1182,16 @@
         <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1199,50 +1199,50 @@
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>158</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="D23" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1250,16 +1250,16 @@
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -1267,17 +1267,17 @@
         <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" ref="E25:E42" si="0">_xlfn.CONCAT("(F) ", B25)</f>
         <v>(F) Testing</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1285,17 +1285,17 @@
         <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
         <v>(F) Wing it!</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1303,17 +1303,17 @@
         <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
         <v>(F) Basic 5th</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -1321,17 +1321,17 @@
         <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D28" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
         <v>(F) Listen to the tones and choose the path that matches</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1339,17 +1339,17 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
         <v>(F) C Chord</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1357,226 +1357,226 @@
         <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
         <v>(F) Listen to the tones and choose the path that matches</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
         <v>(F) Level 1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
         <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D32" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
         <v>(F) Listen to the tones and choose the path that matches</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" t="s">
+        <v>149</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>(F) Level 2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>86</v>
-      </c>
-      <c r="B33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" t="s">
-        <v>153</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="0"/>
-        <v>(F) Level 2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>88</v>
       </c>
       <c r="B34" t="s">
         <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D34" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>(F) Listen to the tones and choose the path that matches</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" t="s">
         <v>150</v>
       </c>
-      <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v>(F) Listen to the tones and choose the path that matches</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" t="s">
-        <v>154</v>
-      </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
         <v>(F) Level 3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D36" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
         <v>(F) Listen to the tones and choose the path that matches</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
         <v>(F) Level 4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
         <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D38" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
         <v>(F) Listen to the tones and choose the path that matches</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
         <v>(F) Level 5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
         <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D40" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
         <v>(F) Listen to the tones and choose the path that matches</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
         <v>(F) Level 6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
         <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>

</xml_diff>